<commit_message>
add new code sample and fix link
</commit_message>
<xml_diff>
--- a/VB/SpreadsheetControl_API_Part03/Documents/DataValidation.xlsx
+++ b/VB/SpreadsheetControl_API_Part03/Documents/DataValidation.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\winforms-spreadsheetcontrol-api-part-3-t231273\VB\SpreadsheetControl_API_Part03\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD916D1-E816-4623-8B30-7AA4FAD9B699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12825"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data validation sample" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Assessment</t>
   </si>
@@ -96,16 +104,19 @@
   </si>
   <si>
     <t>WDU</t>
+  </si>
+  <si>
+    <t>ADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* -#,##0.00 ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,7 +148,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -170,6 +187,12 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -179,36 +202,38 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* -#,##0.00 ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table6" displayName="Table6" ref="H3:H9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table6" displayName="Table6" ref="H3:H9">
   <tableColumns count="1">
-    <tableColumn id="1" name="Department"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Department"/>
   </tableColumns>
-  <tableStyleInfo showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table7" displayName="Table7" ref="B3:F11" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table7" displayName="Table7" ref="B3:F11" headerRowDxfId="2">
   <tableColumns count="5">
-    <tableColumn id="1" name="Employee ID" dataDxfId="1"/>
-    <tableColumn id="2" name="Employee Name"/>
-    <tableColumn id="3" name="Alias"/>
-    <tableColumn id="4" name="Department"/>
-    <tableColumn id="5" name="Hourly Wage" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Employee ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Employee Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Alias"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Department"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Hourly Wage" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -217,10 +242,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -466,39 +491,42 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.29" customWidth="1"/>
-    <col min="3" max="3" width="22.86" customWidth="1"/>
-    <col min="4" max="4" width="5.43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.14" customWidth="1"/>
-    <col min="6" max="6" width="14.57" customWidth="1"/>
+    <col min="1" max="1" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" customWidth="1"/>
+    <col min="3" max="3" width="22.86328125" customWidth="1"/>
+    <col min="4" max="4" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.53125" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33.75" customHeight="1">
+    <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>15</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" ht="17.25" customHeight="1">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -521,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>10115</v>
       </c>
@@ -529,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>8</v>
@@ -540,8 +568,11 @@
       <c r="H4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>10501</v>
       </c>
@@ -561,7 +592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>10709</v>
       </c>
@@ -581,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>10356</v>
       </c>
@@ -601,7 +632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>10401</v>
       </c>
@@ -621,7 +652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <v>10202</v>
       </c>
@@ -641,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>10205</v>
       </c>
@@ -658,7 +689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <v>10403</v>
       </c>
@@ -677,6 +708,7 @@
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>